<commit_message>
Google Sheet support, see README.md for link
</commit_message>
<xml_diff>
--- a/internshipGetter.xlsx
+++ b/internshipGetter.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,19 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,38 +46,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -446,21 +420,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="67" customWidth="1" min="1" max="1"/>
-    <col width="119" customWidth="1" min="2" max="2"/>
+    <col width="72" customWidth="1" min="1" max="1"/>
+    <col width="124" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -481,7 +455,7 @@
           <t>Software Engineering Intern Jobs, Employment in Boston, MA ...</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>https://www.indeed.com/q-software-engineering-intern-l-boston,-ma-jobs.html</t>
         </is>
@@ -493,7 +467,7 @@
           <t>11 Software Engineering Intern jobs in Boston, Massachusetts ...</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/jobs/software-engineering-intern-jobs-boston-ma</t>
         </is>
@@ -505,7 +479,7 @@
           <t>Search and Apply for career opportunities with Bank of America</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>https://campus.bankofamerica.com/opportunities.html</t>
         </is>
@@ -517,7 +491,7 @@
           <t>Internships for students</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>https://www.amazon.jobs/en/teams/internships-for-students</t>
         </is>
@@ -529,7 +503,7 @@
           <t>Internships | NBCUnicareers</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>https://www.nbcunicareers.com/internships</t>
         </is>
@@ -541,7 +515,7 @@
           <t>Internship Opportunities | Careers | Boston Consulting Group</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>https://careers.bcg.com/internship-opportunities</t>
         </is>
@@ -553,7 +527,7 @@
           <t>Students and Grads | Internships at Capital One</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>https://www.capitalonecareers.com/internship-programs</t>
         </is>
@@ -565,7 +539,7 @@
           <t>Students and Graduates | FBIJOBS</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>https://fbijobs.gov/students-and-graduates</t>
         </is>
@@ -577,7 +551,7 @@
           <t>Programs and Internships | Goldman Sachs</t>
         </is>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>https://www.goldmansachs.com/careers/students/programs-and-internships</t>
         </is>
@@ -589,7 +563,7 @@
           <t>NASA Internship Programs - NASA</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>https://www.nasa.gov/learning-resources/internship-programs/</t>
         </is>
@@ -601,7 +575,7 @@
           <t>Internships</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>https://stemgateway.nasa.gov/public/s/explore-opportunities/internships</t>
         </is>
@@ -613,7 +587,7 @@
           <t>MS in Software Engineering Systems | Northeastern University</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>https://graduate.northeastern.edu/program/master-of-science-in-software-engineering-systems-18774/</t>
         </is>
@@ -625,7 +599,7 @@
           <t>Student Programs - CIA</t>
         </is>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>https://www.cia.gov/careers/student-programs/</t>
         </is>
@@ -637,7 +611,7 @@
           <t>Learn About the Boeing Internship Experience and Our Jobs and ...</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>https://jobs.boeing.com/internships</t>
         </is>
@@ -649,7 +623,7 @@
           <t>$19-$29/hr Electrical Engineering Intern Jobs in Boston, MA</t>
         </is>
       </c>
-      <c r="B16" s="2" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>https://www.ziprecruiter.com/Jobs/Electrical-Engineering-Intern/-in-Boston,MA</t>
         </is>
@@ -661,7 +635,7 @@
           <t>Entry Level Opportunities and Jobs - PwC | US Careers</t>
         </is>
       </c>
-      <c r="B17" s="2" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>https://jobs.us.pwc.com/entry-level</t>
         </is>
@@ -673,7 +647,7 @@
           <t>Summer2025-Internships/README-Off-Season.md at dev ...</t>
         </is>
       </c>
-      <c r="B18" s="2" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>https://github.com/SimplifyJobs/Summer2025-Internships/blob/dev/README-Off-Season.md</t>
         </is>
@@ -685,7 +659,7 @@
           <t>Jobs, Student Programs &amp; Internships | JPMorgan Chase &amp; Co.</t>
         </is>
       </c>
-      <c r="B19" s="2" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>https://careers.jpmorgan.com/global/en/students/programs</t>
         </is>
@@ -697,7 +671,7 @@
           <t>GE Aerospace | US Internships</t>
         </is>
       </c>
-      <c r="B20" s="2" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>https://jobs.gecareers.com/aviation/global/en/us-internships</t>
         </is>
@@ -709,7 +683,7 @@
           <t>Ouckah/Summer2025-Internships: Collection of Summer ... - GitHub</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>https://github.com/Ouckah/Summer2025-Internships</t>
         </is>
@@ -721,7 +695,7 @@
           <t>Student Internship Program - Careers</t>
         </is>
       </c>
-      <c r="B22" s="2" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>https://careers.state.gov/interns-fellows/student-internship-program/</t>
         </is>
@@ -733,7 +707,7 @@
           <t>Internships and entry level jobs | Intel Careers</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>https://jobs.intel.com/en/internships</t>
         </is>
@@ -745,7 +719,7 @@
           <t>Careers - Capstone</t>
         </is>
       </c>
-      <c r="B24" s="2" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>https://www.capstoneco.com/careers/</t>
         </is>
@@ -757,7 +731,7 @@
           <t>Internships - Jobs - Careers at Apple</t>
         </is>
       </c>
-      <c r="B25" s="2" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>https://jobs.apple.com/en-us/search?team=internships-STDNT-INTRN</t>
         </is>
@@ -769,40 +743,325 @@
           <t>Undergraduate Internships | Harvard John A. Paulson School of ...</t>
         </is>
       </c>
-      <c r="B26" s="2" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>https://seas.harvard.edu/office-student-career-development/resources-undergraduate-students/undergraduate-internships</t>
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025 Technology Summer Internship - Early Careers (Software or ...</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.wellsfargojobs.com/en/jobs/r-385829/2025-technology-summer-internship-early-careers-software-or-data-engineer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SimplifyJobs/Summer2025-Internships: Collection of ... - GitHub</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://github.com/SimplifyJobs/Summer2025-Internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Internships | Museum of Fine Arts Boston</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.mfa.org/working-at-the-mfa/internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Data and Analytics jobs in Boston, MA | The Muse</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.themuse.com/hiring/location/boston-ma/category/data_analytics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>UMass Cybersecurity Institute</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://infosec.cs.umass.edu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Internships - Red Hat Research</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://research.redhat.com/internships/</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Master of Science in Electrical and Computer Engineering : College ...</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.umass.edu/engineering/academics/ms-electrical-computer-engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Master of Science in Software Development | BU MET</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.bu.edu/met/degrees-certificates/ms-software-development/</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>STUDENT AND GRADUATE OPPORTUNITIES</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.santandercareers.com/students</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Internship Programmes</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://search.jobs.barclays/internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Early Career &amp; Internships | Datadog Careers</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://careers.datadoghq.com/early-careers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Internships | Tesla</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.tesla.com/careers/internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Wayfair Careers | Students</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.aboutwayfair.com/careers/us-students</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Explore Internships at Procter &amp; Gamble</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.pgcareers.com/global/en/internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Students | BNY</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.bnymellon.com/us/en/careers/students.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Student Programs &amp; Early Careers | Siemens Software</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.sw.siemens.com/en-US/careers/student-programs-and-early-careers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Internships - Students and Graduates | Careers | Oracle</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.oracle.com/careers/students-grads/internships/</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Students | Fidelity Careers</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://jobs.fidelity.com/students/</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Careers at BlackRock</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://careers.blackrock.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Internships &amp; Programs | Bain &amp; Company</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://www.bain.com/careers/work-with-us/internships-programs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Campus Reach | Southwest Careers</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://careers.southwestair.com/campus-reach</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Students | Life at Spotify</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.lifeatspotify.com/students</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Internships - IBM Careers</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.ibm.com/careers/internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Early in profession | Microsoft Careers</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://careers.microsoft.com/v2/global/en/students</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Internships – The Estée Lauder Companies Inc.</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.elcompanies.com/en/careers/students/internships</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Summer Internship Opportunities</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://jobs.td.com/en/campus-recruitment/summer-internship-opportunities/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>